<commit_message>
Update TNA Calander-2-08-22 Updated.xlsx
</commit_message>
<xml_diff>
--- a/Docs/TNA Calander-2-08-22 Updated.xlsx
+++ b/Docs/TNA Calander-2-08-22 Updated.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TNA-2-08-2022" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
@@ -387,7 +389,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="94">
   <si>
     <t>Fabric</t>
   </si>
@@ -640,6 +642,36 @@
   </si>
   <si>
     <t>depandant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TNA Date </t>
+  </si>
+  <si>
+    <t>Depandan TNA Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> date diff</t>
+  </si>
+  <si>
+    <t>positive/negative</t>
+  </si>
+  <si>
+    <t>CMS date</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Order Confirmation/ BA/VA Date</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order Confirmation/ BA / VA Date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Date</t>
   </si>
 </sst>
 </file>
@@ -649,7 +681,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -685,8 +717,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -747,6 +786,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -775,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -878,6 +923,30 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1335,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2217,4 +2286,779 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="35"/>
+    <col min="2" max="2" width="20.5703125" style="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="35">
+        <v>1</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="35">
+        <v>2</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="35">
+        <v>3</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="35">
+        <v>4</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="35">
+        <v>5</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="35">
+        <v>6</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>7</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
+        <v>8</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="35">
+        <v>9</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
+        <v>10</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="35">
+        <v>11</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="35">
+        <v>12</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="35">
+        <v>13</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="35">
+        <v>14</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="35">
+        <v>15</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="35">
+        <v>16</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="35">
+        <v>17</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="35">
+        <v>18</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="35">
+        <v>19</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="35">
+        <v>20</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="35">
+        <v>21</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="35">
+        <v>22</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="35">
+        <v>23</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="35">
+        <v>24</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="35">
+        <v>25</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="35">
+        <v>26</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="35">
+        <v>27</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="35">
+        <v>28</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="35">
+        <v>29</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="35">
+        <v>30</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="35">
+        <v>31</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="35">
+        <v>32</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="35">
+        <v>33</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="35">
+        <v>34</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="35">
+        <v>35</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="35">
+        <v>36</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="35">
+        <v>37</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="35">
+        <v>38</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.5703125" style="39" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="39" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="39" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="E2" s="42">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="39">
+        <v>60</v>
+      </c>
+      <c r="E3" s="42">
+        <f>E2-D3</f>
+        <v>44502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="39">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="39">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="39">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C30" s="41"/>
+    </row>
+    <row r="31" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C31" s="41"/>
+    </row>
+    <row r="32" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C32" s="41"/>
+    </row>
+    <row r="33" spans="3:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C33" s="41"/>
+    </row>
+    <row r="34" spans="3:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C34" s="41"/>
+    </row>
+    <row r="35" spans="3:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C35" s="41"/>
+    </row>
+    <row r="36" spans="3:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C36" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>